<commit_message>
New Results from roberta-sms etc
</commit_message>
<xml_diff>
--- a/results/Final_Table/CNN_AES.xlsx
+++ b/results/Final_Table/CNN_AES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karan\Documents\IISc\SEM2\ML\Automatic_Evaluation_Metrics\Official_Repo\IISc-ML-Project\results\Final_Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F450EEEF-46B6-4CB1-ACE1-B1F84422BA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710623F3-F268-4AE7-8097-661748A58640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="360" windowWidth="10224" windowHeight="11976" xr2:uid="{CBC13769-27AD-4DF5-BC08-4B630600A078}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CBC13769-27AD-4DF5-BC08-4B630600A078}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Score</t>
   </si>
@@ -93,14 +93,37 @@
   </si>
   <si>
     <t>SentBERT</t>
+  </si>
+  <si>
+    <t>Spearman Rank Correlation for 2 Datasets</t>
+  </si>
+  <si>
+    <t>Score Metric</t>
+  </si>
+  <si>
+    <t>Summaries</t>
+  </si>
+  <si>
+    <t>Essays</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,10 +151,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,16 +476,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ACE3FA-73CB-46EE-8B93-BFF66993785D}">
-  <dimension ref="F2:J19"/>
+  <dimension ref="F2:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
     <col min="9" max="9" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,7 +525,7 @@
       <c r="H5">
         <v>9.3269155604006906E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>0.61538424199999997</v>
       </c>
       <c r="J5" s="1">
@@ -692,13 +723,13 @@
       <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>0.26315372122443498</v>
       </c>
       <c r="H17" s="1">
         <v>2.28692538192321E-34</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="2">
         <v>0.53577657199999995</v>
       </c>
       <c r="J17" s="1">
@@ -738,11 +769,212 @@
       <c r="J19" s="1">
         <v>1.3900000000000001E-23</v>
       </c>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.67668094941715E-2</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.61538424199999997</v>
+      </c>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0.102188827507858</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.33663348700000001</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.180172319775732</v>
+      </c>
+      <c r="H32" s="6">
+        <v>0.42856114499999998</v>
+      </c>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.25732861378390298</v>
+      </c>
+      <c r="H33" s="6">
+        <v>0.44947218799999999</v>
+      </c>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0.21389133917186001</v>
+      </c>
+      <c r="H34" s="6">
+        <v>0.48756354800000001</v>
+      </c>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0.16030232756682</v>
+      </c>
+      <c r="H35" s="6">
+        <v>0.44036108400000001</v>
+      </c>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0.25307399956494098</v>
+      </c>
+      <c r="H36" s="6">
+        <v>0.43804670200000001</v>
+      </c>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.20347261877414299</v>
+      </c>
+      <c r="H37" s="6">
+        <v>0.48320539099999998</v>
+      </c>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.16889596200715501</v>
+      </c>
+      <c r="H38" s="6">
+        <v>0.36768276</v>
+      </c>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.22895971006059601</v>
+      </c>
+      <c r="H39" s="6">
+        <v>0.41175308500000002</v>
+      </c>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.19876171718671101</v>
+      </c>
+      <c r="H40" s="6">
+        <v>0.413584646</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.178426557580073</v>
+      </c>
+      <c r="H41" s="6">
+        <v>-0.13474971799999999</v>
+      </c>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0.26315372122443498</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.53577657199999995</v>
+      </c>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.25525405987705801</v>
+      </c>
+      <c r="H43" s="6">
+        <v>0.147088571</v>
+      </c>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.11540827300000001</v>
+      </c>
+      <c r="H44" s="6">
+        <v>0.29691668700000001</v>
+      </c>
+      <c r="J44" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I12:L17">
     <sortCondition ref="L12:L17"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="F28:H28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>